<commit_message>
Versión con reportes Word/PDF, Ir a comentario en mantenimiento
</commit_message>
<xml_diff>
--- a/scraping_tools/comentarios_facebook.xlsx
+++ b/scraping_tools/comentarios_facebook.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="355">
   <si>
     <t>nombre</t>
   </si>
@@ -64,6 +64,9 @@
     <t>Andrea Kaulitz</t>
   </si>
   <si>
+    <t>Victor Perez</t>
+  </si>
+  <si>
     <t>Saul Luna</t>
   </si>
   <si>
@@ -103,27 +106,27 @@
     <t>Lunari Tsukishiro</t>
   </si>
   <si>
+    <t>Enrique Romero</t>
+  </si>
+  <si>
     <t>Isco Rod</t>
   </si>
   <si>
+    <t>Hugo Gonzalez</t>
+  </si>
+  <si>
     <t>Charles Saeng</t>
   </si>
   <si>
-    <t>Hugo Gonzalez</t>
+    <t>Cristhian Silva</t>
+  </si>
+  <si>
+    <t>Luis Pignatari</t>
   </si>
   <si>
     <t>Ricardo G. Yzcoa</t>
   </si>
   <si>
-    <t>Cristhian Silva</t>
-  </si>
-  <si>
-    <t>Luis Pignatari</t>
-  </si>
-  <si>
-    <t>Enrique Romero</t>
-  </si>
-  <si>
     <t>María Ortiz</t>
   </si>
   <si>
@@ -142,6 +145,9 @@
     <t>Miguel Simental</t>
   </si>
   <si>
+    <t>Dayimoon Del Rey</t>
+  </si>
+  <si>
     <t>Maritza Herrera</t>
   </si>
   <si>
@@ -157,6 +163,81 @@
     <t>Esme Figueroa</t>
   </si>
   <si>
+    <t>Daniel Fernando Gil García</t>
+  </si>
+  <si>
+    <t>Jorge Ely Jr.</t>
+  </si>
+  <si>
+    <t>Laura Hermione Glu</t>
+  </si>
+  <si>
+    <t>Jose Israel Vega Moreno</t>
+  </si>
+  <si>
+    <t>Billy Goodman Butcher</t>
+  </si>
+  <si>
+    <t>Aldaper Repetto</t>
+  </si>
+  <si>
+    <t>Lucero Almendra Flores Guzmán</t>
+  </si>
+  <si>
+    <t>Yami Chan</t>
+  </si>
+  <si>
+    <t>Jesús Mendivil</t>
+  </si>
+  <si>
+    <t>Pedro Rairan</t>
+  </si>
+  <si>
+    <t>Candela Portales</t>
+  </si>
+  <si>
+    <t>Mario Okazaki</t>
+  </si>
+  <si>
+    <t>Eduardo TL</t>
+  </si>
+  <si>
+    <t>Cäsar G. Rodriguez</t>
+  </si>
+  <si>
+    <t>Vic Montemayor</t>
+  </si>
+  <si>
+    <t>Dan Ortiz</t>
+  </si>
+  <si>
+    <t>Daniel Pic Rey</t>
+  </si>
+  <si>
+    <t>Murasaki Art</t>
+  </si>
+  <si>
+    <t>Carlos Alejandro Rodelo</t>
+  </si>
+  <si>
+    <t>Wanderer Omicozcatl</t>
+  </si>
+  <si>
+    <t>Martin Monjaras</t>
+  </si>
+  <si>
+    <t>Juan Preciado</t>
+  </si>
+  <si>
+    <t>Dom Jose</t>
+  </si>
+  <si>
+    <t>Rosaura Gonzalez</t>
+  </si>
+  <si>
+    <t>Lilliana Aroa Zaraitzu</t>
+  </si>
+  <si>
     <t>Alan Flores</t>
   </si>
   <si>
@@ -166,117 +247,51 @@
     <t>Ray Barron</t>
   </si>
   <si>
-    <t>Daniel Fernando Gil García</t>
-  </si>
-  <si>
-    <t>Jose Israel Vega Moreno</t>
+    <t>Jhon Bitterman</t>
+  </si>
+  <si>
+    <t>Gober Flavio Josefo</t>
+  </si>
+  <si>
+    <t>Cristo Andrea</t>
+  </si>
+  <si>
+    <t>Carlos Garcia</t>
+  </si>
+  <si>
+    <t>Mario Ciprés</t>
+  </si>
+  <si>
+    <t>Jez Cordero</t>
+  </si>
+  <si>
+    <t>Emmanuel Guillermo Giron</t>
   </si>
   <si>
     <t>Ludmila Domé II</t>
   </si>
   <si>
-    <t>Billy Goodman Butcher</t>
-  </si>
-  <si>
-    <t>Aldaper Repetto</t>
-  </si>
-  <si>
-    <t>Jorge Ely Jr.</t>
-  </si>
-  <si>
-    <t>Lucero Almendra Flores Guzmán</t>
-  </si>
-  <si>
-    <t>Yami Chan</t>
-  </si>
-  <si>
-    <t>Jesús Mendivil</t>
-  </si>
-  <si>
-    <t>Pedro Rairan</t>
-  </si>
-  <si>
-    <t>Candela Portales</t>
-  </si>
-  <si>
-    <t>Eduardo TL</t>
-  </si>
-  <si>
-    <t>Mario Okazaki</t>
-  </si>
-  <si>
-    <t>Cäsar G. Rodriguez</t>
-  </si>
-  <si>
-    <t>Vic Montemayor</t>
-  </si>
-  <si>
-    <t>Daniel Pic Rey</t>
+    <t>Mayra Mug</t>
+  </si>
+  <si>
+    <t>JuanMa Santoyo</t>
+  </si>
+  <si>
+    <t>Julián Paradox</t>
+  </si>
+  <si>
+    <t>Christian GuGu</t>
+  </si>
+  <si>
+    <t>Victor Mendez</t>
+  </si>
+  <si>
+    <t>Manuel Granados Vargas</t>
   </si>
   <si>
     <t>Erzebeth Theresa Bathory</t>
   </si>
   <si>
-    <t>Carlos Alejandro Rodelo</t>
-  </si>
-  <si>
-    <t>Wanderer Omicozcatl</t>
-  </si>
-  <si>
-    <t>Martin Monjaras</t>
-  </si>
-  <si>
-    <t>Juan Preciado</t>
-  </si>
-  <si>
-    <t>Dom Jose</t>
-  </si>
-  <si>
-    <t>Rosaura Gonzalez</t>
-  </si>
-  <si>
-    <t>Lilliana Aroa Zaraitzu</t>
-  </si>
-  <si>
-    <t>Jhon Bitterman</t>
-  </si>
-  <si>
-    <t>Gober Flavio Josefo</t>
-  </si>
-  <si>
-    <t>Cristo Andrea</t>
-  </si>
-  <si>
-    <t>Mario Ciprés</t>
-  </si>
-  <si>
-    <t>Jez Cordero</t>
-  </si>
-  <si>
-    <t>Carlos Garcia</t>
-  </si>
-  <si>
-    <t>Emmanuel Guillermo Giron</t>
-  </si>
-  <si>
-    <t>Mayra Mug</t>
-  </si>
-  <si>
-    <t>JuanMa Santoyo</t>
-  </si>
-  <si>
-    <t>Julián Paradox</t>
-  </si>
-  <si>
-    <t>Christian GuGu</t>
-  </si>
-  <si>
-    <t>Victor Mendez</t>
-  </si>
-  <si>
-    <t>Manuel Granados Vargas</t>
-  </si>
-  <si>
     <t>Daniel Corona</t>
   </si>
   <si>
@@ -292,37 +307,40 @@
     <t>Solecillo SinNombre</t>
   </si>
   <si>
+    <t>Karen VF</t>
+  </si>
+  <si>
     <t>Oscar</t>
   </si>
   <si>
     <t>Sandy Gasca</t>
   </si>
   <si>
-    <t>Karen VF</t>
+    <t>Gabriel Rodríguez</t>
+  </si>
+  <si>
+    <t>Janis Silva</t>
   </si>
   <si>
     <t>Edward Nashton</t>
   </si>
   <si>
-    <t>Gabriel Rodríguez</t>
-  </si>
-  <si>
-    <t>Janis Silva</t>
+    <t>Ribay Hernández</t>
   </si>
   <si>
     <t>Norman Medina</t>
   </si>
   <si>
-    <t>Ribay Hernández</t>
-  </si>
-  <si>
     <t>Leonardo Gael</t>
   </si>
   <si>
+    <t>Marta Palestina Manriquez Morales</t>
+  </si>
+  <si>
+    <t>Rojas Angel</t>
+  </si>
+  <si>
     <t>Ignacio Nieto</t>
-  </si>
-  <si>
-    <t>Rojas Angel</t>
   </si>
   <si>
     <t>Lo importante no es la edad, es cómo te sientas aquí en tu corazón, cuate.
@@ -372,6 +390,22 @@
   <si>
     <t>Milo Thatch
 a partir de los 45 tu calidad de esperma baja y tus hijos son propensos a tener miles de enfermedades, muchos más problemas que con una mamá "vieja"</t>
+  </si>
+  <si>
+    <t>Milo Thatch
+La calidad de ese esperma es basura, intenta tener un hijo a esa edad y te va venir con más problemas, no creas que la edad no te afecta a ti en eso</t>
+  </si>
+  <si>
+    <t>Andrea Kaulitz
+probablemente, eso sucede cuando has llevado una vida sedentaria, con una mala alimentación y cero ejercicio. Así es muy probable lo que mencionas.</t>
+  </si>
+  <si>
+    <t>Milo Thatch
+no realmente, por si solo ya ocurre ese declive. Si bien no dejas de producir esperma del todo a lo largo de tu vida, tampoco es el de mejor calidad</t>
+  </si>
+  <si>
+    <t>Andrea Kaulitz
+no tiene caso explicárselo, es de los que piensan que las mujeres después de los 30 ya no sirven mientras que el aunque tenga 60 es todo un semental y está en su mejor época</t>
   </si>
   <si>
     <t>Aunque no estemos calvos, claramente estamos muy lejos de ser adolescentes, pero coincido que muchos piensan que "son los nuevos 20's" nomms no, ya metele tu plan de retiro, ya hazte cargo de tus hijos, ya preocúpate por tu salud wey jajajaja</t>
@@ -436,25 +470,25 @@
     <t>atte: el güey que está calvo desde los 25</t>
   </si>
   <si>
+    <t>Ya somos adultos we no mms.</t>
+  </si>
+  <si>
     <t>Que maduren las frutas alv</t>
   </si>
   <si>
+    <t>Como oveja</t>
+  </si>
+  <si>
     <t>Jajaja el mal del Puer Aethernus... XD</t>
   </si>
   <si>
-    <t>Como oveja</t>
+    <t>Cuenta en decadencia, estaba bien perrona esta cuenta, qué pasó?</t>
+  </si>
+  <si>
+    <t>Tengo 34 y vengo a desmentir al vejestorio este. A mi edad ya estoy más cerca del descanso eterno que de la adolescencia.</t>
   </si>
   <si>
     <t>Para los 30 uno ya lleva 12 años siendo adulto</t>
-  </si>
-  <si>
-    <t>Cuenta en decadencia, estaba bien perrona esta cuenta, qué pasó?</t>
-  </si>
-  <si>
-    <t>Tengo 34 y vengo a desmentir al vejestorio este. A mi edad ya estoy más cerca del descanso eterno que de la adolescencia.</t>
-  </si>
-  <si>
-    <t>Ya somos adultos we no mms.</t>
   </si>
   <si>
     <t>Uno</t>
@@ -489,6 +523,15 @@
 ok gordita</t>
   </si>
   <si>
+    <t>Miguel Simental
+también eres gorda, imbecil. O me vas a decir que esos cachetes son de puro aire??? Mirate al espejo primero.</t>
+  </si>
+  <si>
+    <t>Dayimoon Del Rey
+no se comparan los cachetes y la panzota colgadota del tipo
+y si pero gorda me la pones bb.</t>
+  </si>
+  <si>
     <t>Conozco a uno de 47 bien desubicado correteando niñas de 18... lo gracioso, es que según los rabos verdes, se supone que les tengo envidia...de que a mi los calvos +35 "ya no me corretean" jajajjaaajaj</t>
   </si>
   <si>
@@ -507,33 +550,23 @@
 jajajaj estaba buscando está referencia</t>
   </si>
   <si>
-    <t>Entonces... ¿te vas a salir de casa de tus papás hasta los 45?</t>
-  </si>
-  <si>
-    <t>Alan Flores
-Dos de mis tíos ya van para esa edad y nada que se van</t>
-  </si>
-  <si>
-    <t>Alan Flores
-si dios me da vida hasta me quedo con la casa</t>
-  </si>
-  <si>
     <t>Entiendo que dicho por gente como el Dun ya dan ganas pero de haber hecho de todo y ser exitoso antes de los 25 a como dé lugar por el miedo a terminar como él o su ovino...</t>
   </si>
   <si>
+    <t>Que chistosos son los ancianos calvos que se creen jóvenes jajajajajajajajajajaja, mejor vayan a revisarse la próstata</t>
+  </si>
+  <si>
+    <t>Jorge Ely Jr.
+Dejalos que estan en su prime dicen jaja</t>
+  </si>
+  <si>
     <t>Heyyy los 50 primeros años, de la infancia son los más difíciles</t>
   </si>
   <si>
-    <t>"Aún no estoy listo para algo serio"</t>
-  </si>
-  <si>
     <t>como yo me siento a mi avanzada edad de 33 años viendo a la chaviza en sus 20s...</t>
   </si>
   <si>
     <t>A los 30 sientes que a los 20 eras un tonto inexperto, a los 45 sientes que a los 30 eras un tonto, a los 60 piensas que a los 45 no tenías experiencia. A los 95 te ríes de pésimos consejos de vida que dabas a los 80 años.</t>
-  </si>
-  <si>
-    <t>Que chistosos son los ancianos calvos que se creen jóvenes jajajajajajajajajajaja, mejor vayan a revisarse la próstata</t>
   </si>
   <si>
     <t>Entonces por eso no trabajan, porque sería trabajo infantil</t>
@@ -556,25 +589,28 @@
 , eso no tiene nada que ver con decir que a los 30 aún tienes aspecto de niño.</t>
   </si>
   <si>
+    <t>Pues es que a los 30 real estás en tu pick de la vida humana, si ya estás dado alv checa tu estilo de vida</t>
+  </si>
+  <si>
     <t>Gente que no merece que le tapen el nombre</t>
   </si>
   <si>
-    <t>Pues es que a los 30 real estás en tu pick de la vida humana, si ya estás dado alv checa tu estilo de vida</t>
-  </si>
-  <si>
     <t>47 años tiene el bebé que aun depende de sus papis.</t>
   </si>
   <si>
     <t>El problema de haber nacido en los 90s</t>
   </si>
   <si>
+    <t>Porque la gente niega mucho el estar envejeciendo?</t>
+  </si>
+  <si>
     <t>puro chavoruko en los comentarios</t>
   </si>
   <si>
+    <t>Estos son los que dicen que las mujeres a lo 25 ya están viejas y acabadas</t>
+  </si>
+  <si>
     <t>Me pregunto que tendrá ese compa para pensar eso, a mis 21 años, me siento como si y atuviera 50 (sigo igual de pndjo)</t>
-  </si>
-  <si>
-    <t>Aspecto de niño ? No manchen me dio asco leer eso jajaja</t>
   </si>
   <si>
     <t>35 añitos tiene la bendi</t>
@@ -625,6 +661,17 @@
 Depende de la persona, hay gente que a sus 40 se sienten bien y hay weyes de 20 ya bien jodidos y es por multiples circunstancias en la vida</t>
   </si>
   <si>
+    <t>Entonces... ¿te vas a salir de casa de tus papás hasta los 45?</t>
+  </si>
+  <si>
+    <t>Alan Flores
+Dos de mis tíos ya van para esa edad y nada que se van</t>
+  </si>
+  <si>
+    <t>Alan Flores
+si dios me da vida hasta me quedo con la casa</t>
+  </si>
+  <si>
     <t>Ya te vimos, dumentio jajajaja</t>
   </si>
   <si>
@@ -634,16 +681,19 @@
     <t>De por sí el varón madura más tardíamente, y por si fuera poco, esta epoca no nos fuerza a madurar antes, como nuestros abuelos, que eran señores hechos y derechos a los 25.</t>
   </si>
   <si>
+    <t>Soy ese ( yo con 33)</t>
+  </si>
+  <si>
     <t>Este we malinterpretó el seguir siendo jovial con ser inmaduro...</t>
   </si>
   <si>
     <t>40 años tiene la criatura</t>
   </si>
   <si>
-    <t>Soy ese ( yo con 33)</t>
-  </si>
-  <si>
     <t>Oveja eres tu?</t>
+  </si>
+  <si>
+    <t>"Aún no estoy listo para algo serio"</t>
   </si>
   <si>
     <t>Annie Muñiza
@@ -668,6 +718,9 @@
     <t>Eso le dijo a su mamá cuando lo intentó sacar de la casa o cobrarle renta.</t>
   </si>
   <si>
+    <t>Aspecto de niño ? No manchen me dio asco leer eso jajaja</t>
+  </si>
+  <si>
     <t>Si a mis 33 ya me rechinan las rodillas XD</t>
   </si>
   <si>
@@ -681,378 +734,411 @@
   </si>
   <si>
     <t>Gente que no merece que le tapen el Nombre</t>
+  </si>
+  <si>
+    <t>Maximiliano Monroy Sánchez</t>
   </si>
   <si>
     <t>Oscar
 Soy un bebé.</t>
   </si>
   <si>
-    <t>Maximiliano Monroy Sánchez</t>
-  </si>
-  <si>
     <t>Gabriel Rodríguez
 Basado.</t>
   </si>
   <si>
+    <t>La vida de un hombre empieza a los 40 pleb</t>
+  </si>
+  <si>
     <t>¿ Esto que tiene de mamador ?</t>
   </si>
   <si>
-    <t>La vida de un hombre empieza a los 40 pleb</t>
-  </si>
-  <si>
     <t>Cómo dice el dun, la vida de un hombre empieza a los 40 xd</t>
+  </si>
+  <si>
+    <t>Soy una escritora niña de 62 años</t>
+  </si>
+  <si>
+    <t>"uno"</t>
   </si>
   <si>
     <t>Arely
 Naaaa</t>
   </si>
   <si>
-    <t>"uno"</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/MamadoresLiterarios?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2MjA0MzQxMzI1NDQ2OQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/pepe.estopellan.1?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3Mjk4ODU0OTE3NDA1MjU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/MamadoresLiterarios?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExNzMwMTUzMDc2MzI1MDY%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/iZeveNN?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyNDA1NzIxMDQyOTg0NDY%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/luis.roberto.92560?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMDI1OTY2NTg2OTMwNw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chaneke.valiant?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk5ODQwMzgyMjUwMzg1OQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/ale.velasko?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExODIxMzI1MTY5OTEyOTQ%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/2maryu2?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwODYyNjQyMzM1NjMyMzA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/paolamontemayor?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0MjY1Nzg5NjQzNjM4OTg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/milopenamx?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMDYyMzgyMjM2NjUwMg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/donajialejandra.torresnoriega.3?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwODMwOTAzMzA1MTMzNzI%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100087514184597&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI5MzczNzE4NDEyMjczNjM4&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/greynas?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzNjEwOTU5Mzg1MTAzMjc%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/andrea.t.kaulitz?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0Mzc4MDg5NDc2NDc0NTE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/dc.maldonado.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIwNzE0MzcyMTAwMjEyODM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/jessy.k.moran.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE1ODQxMDYxMjU2MTI0MTg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100009293364331&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExMDUwNzQ1OTgwOTE1NzM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/jessy.k.moran.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0NDc0Nzg1NDY2Mjg5ODU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100009293364331&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjk3MjgzNzE4NjM1ODM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chacon.sustaita.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1MDE4ODY1MTIyMjQ0OA%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/carolina.martinez.500271?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4MzQxMjU4OTQxMDM1NTc%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100010713093534&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE1ODE4NjkzMjU3OTE4OTU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/felix.beltranalvarado.1?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMjY0NTgxMjIyNTU2Mg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/esteban.acostaavila.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MTE0MTEyODM1NDk1MDU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/oswaldo.herreraquintana?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyNDcwNDM3MDAxNzUxOTk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vrensh.torresgii?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk1NTUxMzM0NzQ2MTI4NzA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/auespn?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY0NDE1NDk1ODQ0OTE5Mg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/elartistaantes.conocidocomoklaha?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3OTQwOTcwNjgxMTU2NTU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/MamadoresLiterarios?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0NzY1NTY4NDI2ODU5NTM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/lunarimoonmun.dsun.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMzAxMTA3ODkwMjc2NDk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/luis.roberto.92560?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY4MDExNDcyMTA2NjEwNg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/isco.rod.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3MDMxMDczNzcwODE2OTc%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/charles.saeng.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk4NTUyNjk5MTQ1ODg5MDE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=61554507827877&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY4NjQ0ODMxMzg0NjMxNg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/yzcoa42?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU4Njc2MDE4Nzc1NzgwNQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/kriztianSilva?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4NTg1MjQ4NzgyNzg4MjE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/luis.supertramp.9?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU4NzA2MDA5Mzc1NDgwOQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/enrique.romero.52203?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI5MjcyNzIwNDQxNDYyNjA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/luzmaria.ortiz.90260?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjg5MTMzMTU4NTc5OTE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=61556271031703&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNTEyMzY4NjY4OTY5MzM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/d.Alain.Garcia?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU2NjMwMjM1NjQ5NDUyMw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/paolamontemayor?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMzQ3MDM4OTUyMTA3NTE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/lemon.pie741?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY5OTI2MTM2OTkxODY0Ng%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/sandy.allthehate?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk2ODExODkyNzUyNTA0MTU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/miguel.simental.02?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE5MDc1OTcyNjMzOTczNjc%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/sandy.allthehate?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4OTE3MTUyNjE2NTM4Mzc%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/miguel.simental.02?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MDk3MDMyNTcwNDgzNzE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/maritza.herrera.9440?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMTAxNjUwMzcxNDM5NTA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/rosario.carbajalrodriguez?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMDM4MTg4OTMxNTA2Mw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/erion.hernandez.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIwNjEzNTA4MjQzMzkzMzU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/andres.ramireztrujillo.146?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIxMDc5MDMxODYzMTg4Njg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100007259985243&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3NDc2OTQxMTkyMTE0MTM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/alan.flores.547389?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2NTg0ODQ1Mjc1Mjc4Nw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100062097249954&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY5NjMyOTM0Mjg4NDY5NQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/ray.barronol.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU0NjUzNTI2NDg1MDQ2NA%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/danielfernando.gilgarcia?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExODE0Mzk1NzM5OTUwNjU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/joseisrael.vegamoreno?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY3NTE0ODQ3NTExMTAxMw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/ludmila.domeii?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY4MDA2MzI2ODA4MDA4Mw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/better.call.william.13?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMTc1MzIyMDM2NjI2NTA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/manuel.espinola.10004?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY3MzUzNjY4ODc5MDIxNg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100079943478565&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NDg0NzcyNDEyNjg4NQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/luzlmendra.floresguzman?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzMTExNDczNTk5Nzk2Njg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/dayami.chavez?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MjcyODg3NjUzNzYyMDM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/jesus.mendivil.75873?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzQyNzE4NDI3Nzk3MTc3ODA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/pedro.rairan?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3OTczODUzNDA4MzAxMjk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/erion.hernandez.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExOTA3MTU1ODIyMDI2MTE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100014503038383&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzNDQ4MDI5MDAxNDY3NDM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/edduardoTL?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMTE1MjY1NjcyNzc5MTQ%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/mario.sierra.1272?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3ODExOTk3NDU3NzU2NDk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/30MAR90?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMTIxODU5NzMyMjQzMDQ%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vic.montemayor.27?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0MTI1NTMxMTkxMjcyMjE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/daniel.pic.rey?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MDQwNTA2NTM5MzA1NDk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/erion.hernandez.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcxMzg1Mjg3NzY2ODAyMQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/blooding.countess?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjg5MDc0Njg2NjU0NzI%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/Charlie.Rodelo?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3MDI2ODgzMzczMDA5MDg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/wanderer.omicozcatluchiha?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMDk0NjU1MTQwMTIwMzk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/martin.monjaras.71?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDkxNTYxOTA0NTMxNDY%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/wanderer.omicozcatluchiha?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk5Mzk3Njg5Mjg5NzYzNw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/israel.salvador.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzNTI3NjE5NjI2ODEzNjg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/ajosephhb?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjY0MDAyMDYwOTQzNjA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/esteban.acostaavila.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3NTI4OTg0MDU2NDA2ODA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/rosaura.gonzalez.54?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzUxNDIwODAxNDk2MzYxOA%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/esteban.acostaavila.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDMwMjM2MTc5MjQ0OTU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/rosaura.gonzalez.54?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzUzOTkwODY2ODkxNDg3Nw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/israel.salvador.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2NzgwNjk2MjUzOTQxNg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/LilianaZaraitzu?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzkyMjQxODU5OTg5MzE2Ng%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/jhonatan.solis.5680?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMDc2NzU0ODc0MjIyOTk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/elgobersuculento?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzMxOTE4NzE5MjQyOTQ3MTU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/cristofor?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzQ4OTMxNTgzNDE3MTkwMA%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/mcipres1?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0Mjc4MTI4ODUyNDM3MTg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/jezkib?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMzQ3NzUyOTU0MjAwODc%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/carlos.garcia.679739?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE1OTUxMjM5MTQ0MTUxNDA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/emmanuel.guillermogiron?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0NjAyODY1NjQzMjI0Nzk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/mayra.mug?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDY3NzAyMDczMjAzMzM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/manu.santoyo.9?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzMzExNDIwMTE0ODE0MjQ%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/paradoxografo?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY3ODkzNjgyMTUyNTM2Mg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/christian.gugu.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0NjI4MTE3MzgwMjM5ODM%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vickh.mv?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk3OTM0NTY4NjQwNDEwOTA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/mgranadosv?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzczNDgwOTQzNTU0MjcwNg%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/daniel.r.corona.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk1Mzk1NDU2MjYwOTQ3MDE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/rockdrigo.orochi?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMTU0NzA0MjY4MzA3MTU%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/ElPincheJonathan?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzUyNjEzOTA4Mzg5NjkzNA%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/angel.toriz.457517?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyNDM3MTczMTA0MjM1MDg%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/SolecilloSinNombre?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExOTQwMzc3OTU3OTkzMTE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100094297117790&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDIxMTU5NjQwMzE5Njk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/sandiacarbonizada?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzYwMjQ3ODExMjgzODQyOQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/VafloK?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMDEyNjIwOTE3MjQzNzE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/profile.php?id=100015749924172&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NjQ3NTExMzk2MDAwMA%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/gabriel.rodriguezramirez.75?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NjIyNDcxNzI1ODI1OQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/janis.silva.290814?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDE4MTE0NTQ1NDU4Mjk%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/norman.medina.508639?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIwMjE3OTI5NjgzNDg1MjE%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/TzaXaguum?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU3NjQ4Nzg0MjE0NDU4OQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/leonardo.gael.9674?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4Mjg0NDc2MjQzNjc5MTA%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/ignacio.garcianieto?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcxODgxOTM2NzQ3NzQ4Mw%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/poxood?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY0NDEzOTAxMTc5Mjc4OQ%3D%3D&amp;__cft__[0]=AZWpOVqAw6e3vP35tIezy5Gkn1p5EEgw8v6WPzqhw3xv-HHGMojlWq8YMo7RsHapH08ShaR4n7Pta3JKGsO-KbZbl-U08pYFxIaK2ryzAJd4wRPpizoMovbi8wmFTVeWh4kKm612DsIuRadP_fBFyIWlypiWID6pbF5dw6RA0sndZA&amp;__tn__=R]-R</t>
+    <t>https://www.facebook.com/MamadoresLiterarios?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2MjA0MzQxMzI1NDQ2OQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/pepe.estopellan.1?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3Mjk4ODU0OTE3NDA1MjU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/MamadoresLiterarios?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExNzMwMTUzMDc2MzI1MDY%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/iZeveNN?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyNDA1NzIxMDQyOTg0NDY%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/luis.roberto.92560?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMDI1OTY2NTg2OTMwNw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chaneke.valiant?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk5ODQwMzgyMjUwMzg1OQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ale.velasko?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExODIxMzI1MTY5OTEyOTQ%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/2maryu2?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwODYyNjQyMzM1NjMyMzA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/paolamontemayor?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0MjY1Nzg5NjQzNjM4OTg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/milopenamx?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMDYyMzgyMjM2NjUwMg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/donajialejandra.torresnoriega.3?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwODMwOTAzMzA1MTMzNzI%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100087514184597&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI5MzczNzE4NDEyMjczNjM4&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/greynas?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzNjEwOTU5Mzg1MTAzMjc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/andrea.t.kaulitz?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0Mzc4MDg5NDc2NDc0NTE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/diosyato?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NTcyMTI2MzkwNjYwNg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/milopenamx?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIxNDU3MTg0NDkyNjA5NTM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/andrea.t.kaulitz?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2MzQyMDI4MzMzNjI1OQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/greynas?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNTIyNDY2MzAxMjg5NDc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/dc.maldonado.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIwNzE0MzcyMTAwMjEyODM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/jessy.k.moran.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE1ODQxMDYxMjU2MTI0MTg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100009293364331&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExMDUwNzQ1OTgwOTE1NzM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/jessy.k.moran.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0NDc0Nzg1NDY2Mjg5ODU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100009293364331&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjk3MjgzNzE4NjM1ODM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chacon.sustaita.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1MDE4ODY1MTIyMjQ0OA%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/carolina.martinez.500271?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4MzQxMjU4OTQxMDM1NTc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100010713093534&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE1ODE4NjkzMjU3OTE4OTU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/felix.beltranalvarado.1?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMjY0NTgxMjIyNTU2Mg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/esteban.acostaavila.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MTE0MTEyODM1NDk1MDU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/oswaldo.herreraquintana?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyNDcwNDM3MDAxNzUxOTk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vrensh.torresgii?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk1NTUxMzM0NzQ2MTI4NzA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/auespn?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY0NDE1NDk1ODQ0OTE5Mg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/elartistaantes.conocidocomoklaha?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3OTQwOTcwNjgxMTU2NTU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/MamadoresLiterarios?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0NzY1NTY4NDI2ODU5NTM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/lunarimoonmun.dsun.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMzAxMTA3ODkwMjc2NDk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/luis.roberto.92560?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY4MDExNDcyMTA2NjEwNg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/enrique.romero.52203?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI5MjcyNzIwNDQxNDYyNjA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/isco.rod.7?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3MDMxMDczNzcwODE2OTc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=61554507827877&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY4NjQ0ODMxMzg0NjMxNg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/charles.saeng.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk4NTUyNjk5MTQ1ODg5MDE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/kriztianSilva?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4NTg1MjQ4NzgyNzg4MjE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/luis.supertramp.9?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU4NzA2MDA5Mzc1NDgwOQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/yzcoa42?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU4Njc2MDE4Nzc1NzgwNQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/luzmaria.ortiz.90260?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjg5MTMzMTU4NTc5OTE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=61556271031703&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNTEyMzY4NjY4OTY5MzM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/d.Alain.Garcia?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU2NjMwMjM1NjQ5NDUyMw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/paolamontemayor?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMzQ3MDM4OTUyMTA3NTE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/lemon.pie741?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY5OTI2MTM2OTkxODY0Ng%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/sandy.allthehate?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk2ODExODkyNzUyNTA0MTU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/miguel.simental.02?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE5MDc1OTcyNjMzOTczNjc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/sandy.allthehate?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4OTE3MTUyNjE2NTM4Mzc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/miguel.simental.02?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MDk3MDMyNTcwNDgzNzE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/dayana.chavez.1441?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk0NDM0MTcxODI0NTIwMDQ%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/miguel.simental.02?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzQ0ODYyNTYyMDQ5MzQzODY%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/maritza.herrera.9440?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMTAxNjUwMzcxNDM5NTA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/rosario.carbajalrodriguez?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcwMDM4MTg4OTMxNTA2Mw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/erion.hernandez.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIwNjEzNTA4MjQzMzkzMzU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/andres.ramireztrujillo.146?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIxMDc5MDMxODYzMTg4Njg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100007259985243&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3NDc2OTQxMTkyMTE0MTM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/danielfernando.gilgarcia?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExODE0Mzk1NzM5OTUwNjU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100079943478565&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NDg0NzcyNDEyNjg4NQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/laura.garcialuna.315?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE2MjY2MzA4MDQ2ODY5NTc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/joseisrael.vegamoreno?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY3NTE0ODQ3NTExMTAxMw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/better.call.william.13?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMTc1MzIyMDM2NjI2NTA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/manuel.espinola.10004?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY3MzUzNjY4ODc5MDIxNg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/luzlmendra.floresguzman?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzMTExNDczNTk5Nzk2Njg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/dayami.chavez?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MjcyODg3NjUzNzYyMDM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/jesus.mendivil.75873?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzQyNzE4NDI3Nzk3MTc3ODA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/pedro.rairan?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3OTczODUzNDA4MzAxMjk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/erion.hernandez.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExOTA3MTU1ODIyMDI2MTE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100014503038383&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzNDQ4MDI5MDAxNDY3NDM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/mario.sierra.1272?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3ODExOTk3NDU3NzU2NDk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/edduardoTL?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMTE1MjY1NjcyNzc5MTQ%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/30MAR90?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMTIxODU5NzMyMjQzMDQ%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vic.montemayor.27?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0MTI1NTMxMTkxMjcyMjE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/dan.ortiz.31542?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk2OTU2NjY1NTcxNzc5Nzk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daniel.pic.rey?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0MDQwNTA2NTM5MzA1NDk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=61567004950489&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1OTM1NDk3MzM4NTg4Ng%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/erion.hernandez.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcxMzg1Mjg3NzY2ODAyMQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Charlie.Rodelo?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3MDI2ODgzMzczMDA5MDg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/wanderer.omicozcatluchiha?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMDk0NjU1MTQwMTIwMzk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/martin.monjaras.71?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDkxNTYxOTA0NTMxNDY%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/wanderer.omicozcatluchiha?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk5Mzk3Njg5Mjg5NzYzNw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/israel.salvador.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzNTI3NjE5NjI2ODEzNjg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ajosephhb?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjY0MDAyMDYwOTQzNjA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/esteban.acostaavila.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE3NTI4OTg0MDU2NDA2ODA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/rosaura.gonzalez.54?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzUxNDIwODAxNDk2MzYxOA%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/esteban.acostaavila.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDMwMjM2MTc5MjQ0OTU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/rosaura.gonzalez.54?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzUzOTkwODY2ODkxNDg3Nw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/israel.salvador.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2NzgwNjk2MjUzOTQxNg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/LilianaZaraitzu?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzkyMjQxODU5OTg5MzE2Ng%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/alan.flores.547389?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY2NTg0ODQ1Mjc1Mjc4Nw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100062097249954&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY5NjMyOTM0Mjg4NDY5NQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ray.barronol.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU0NjUzNTI2NDg1MDQ2NA%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/jhonatan.solis.5680?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMDc2NzU0ODc0MjIyOTk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/elgobersuculento?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzMxOTE4NzE5MjQyOTQ3MTU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/cristofor?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzQ4OTMxNTgzNDE3MTkwMA%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/carlos.garcia.679739?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE1OTUxMjM5MTQ0MTUxNDA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/mcipres1?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0Mjc4MTI4ODUyNDM3MTg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/jezkib?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMzQ3NzUyOTU0MjAwODc%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/emmanuel.guillermogiron?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzI0NjAyODY1NjQzMjI0Nzk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ludmila.domeii?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY4MDA2MzI2ODA4MDA4Mw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/mayra.mug?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDY3NzAyMDczMjAzMzM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/manu.santoyo.9?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEzMzExNDIwMTE0ODE0MjQ%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/paradoxografo?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY3ODkzNjgyMTUyNTM2Mg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/christian.gugu.2025?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE0NjI4MTE3MzgwMjM5ODM%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vickh.mv?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk3OTM0NTY4NjQwNDEwOTA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/mgranadosv?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzczNDgwOTQzNTU0MjcwNg%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/blooding.countess?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMjg5MDc0Njg2NjU0NzI%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/daniel.r.corona.5?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2Xzk1Mzk1NDU2MjYwOTQ3MDE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/rockdrigo.orochi?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMTU0NzA0MjY4MzA3MTU%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ElPincheJonathan?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzUyNjEzOTA4Mzg5NjkzNA%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/angel.toriz.457517?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyNDM3MTczMTA0MjM1MDg%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/SolecilloSinNombre?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzExOTQwMzc3OTU3OTkzMTE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/VafloK?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwMDEyNjIwOTE3MjQzNzE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100094297117790&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDIxMTU5NjQwMzE5Njk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/sandiacarbonizada?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzYwMjQ3ODExMjgzODQyOQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/gabriel.rodriguezramirez.75?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NjIyNDcxNzI1ODI1OQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/janis.silva.290814?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEwNDE4MTE0NTQ1NDU4Mjk%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100015749924172&amp;comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY1NjQ3NTExMzk2MDAwMA%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/TzaXaguum?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzU3NjQ4Nzg0MjE0NDU4OQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/norman.medina.508639?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzIwMjE3OTI5NjgzNDg1MjE%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/leonardo.gael.9674?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzE4Mjg0NDc2MjQzNjc5MTA%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/martapalestina.manriquezmorales?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzEyMTc5ODAwMTMyODQwNzI%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/poxood?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzY0NDEzOTAxMTc5Mjc4OQ%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ignacio.garcianieto?comment_id=Y29tbWVudDoxMjExMjc4MDYwNTU0MjI2XzcxODgxOTM2NzQ3NzQ4Mw%3D%3D&amp;__cft__[0]=AZU4kUu8RToMLE-q2pa1Rm0cWGLbhbI_hwC4FCXDWRncSgFULrRjTh6G5W4H8qTM3_UJVIoTmYF2Xck0mQrPdkFagt5UFnm8ELUrows5y8iAOK1p28rlo5l0aOzx3_9kKAgNkarsQU2TwPywtQvEaEtY5mksQPxh3EnxY0m5r7_pOQ&amp;__tn__=R]-R</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1445,10 +1531,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1456,10 +1542,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1467,10 +1553,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1478,10 +1564,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1489,10 +1575,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1503,7 +1589,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1511,10 +1597,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1522,10 +1608,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1533,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1544,10 +1630,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1555,10 +1641,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1566,10 +1652,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1577,10 +1663,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1588,10 +1674,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1599,1110 +1685,1220 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B70" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B71" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B79" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B80" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B81" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B82" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B83" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B84" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B85" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B88" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B91" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B92" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B94" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B95" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B97" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>313</v>
+        <v>329</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>315</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B105" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>317</v>
+        <v>333</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B106" t="s">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>318</v>
+        <v>334</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B107" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B109" t="s">
-        <v>141</v>
+        <v>215</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B110" t="s">
-        <v>97</v>
+        <v>216</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B111" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B112" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B113" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>325</v>
+        <v>341</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B114" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>326</v>
+        <v>342</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B115" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>327</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>98</v>
+      </c>
+      <c r="B116" t="s">
+        <v>99</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>99</v>
+      </c>
+      <c r="B117" t="s">
+        <v>222</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>100</v>
+      </c>
+      <c r="B118" t="s">
+        <v>101</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>101</v>
+      </c>
+      <c r="B119" t="s">
+        <v>223</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
         <v>102</v>
       </c>
-      <c r="B116" t="s">
-        <v>213</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>328</v>
+      <c r="B120" t="s">
+        <v>151</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>103</v>
+      </c>
+      <c r="B121" t="s">
+        <v>224</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>104</v>
+      </c>
+      <c r="B122" t="s">
+        <v>225</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>105</v>
+      </c>
+      <c r="B123" t="s">
+        <v>226</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124" t="s">
+        <v>227</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>107</v>
+      </c>
+      <c r="B125" t="s">
+        <v>228</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>108</v>
+      </c>
+      <c r="B126" t="s">
+        <v>229</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -2822,6 +3018,16 @@
     <hyperlink ref="C114" r:id="rId113"/>
     <hyperlink ref="C115" r:id="rId114"/>
     <hyperlink ref="C116" r:id="rId115"/>
+    <hyperlink ref="C117" r:id="rId116"/>
+    <hyperlink ref="C118" r:id="rId117"/>
+    <hyperlink ref="C119" r:id="rId118"/>
+    <hyperlink ref="C120" r:id="rId119"/>
+    <hyperlink ref="C121" r:id="rId120"/>
+    <hyperlink ref="C122" r:id="rId121"/>
+    <hyperlink ref="C123" r:id="rId122"/>
+    <hyperlink ref="C124" r:id="rId123"/>
+    <hyperlink ref="C125" r:id="rId124"/>
+    <hyperlink ref="C126" r:id="rId125"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>